<commit_message>
got parts of combined MCR/expression heatmap
</commit_message>
<xml_diff>
--- a/test_scripts/all_bins_RNA/normalized_covg_bins_RNA.xlsx
+++ b/test_scripts/all_bins_RNA/normalized_covg_bins_RNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgalambos/Documents/GitHub/meta-omics/test_scripts/all_bins_RNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{07D807DF-7C1D-A743-B795-42DD6F4CA76C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D3C982-0603-634A-951F-8A74EABBAC2E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="14400" windowHeight="16100"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="normalized" sheetId="1" r:id="rId1"/>
@@ -127,6 +127,9 @@
     <t>Thiotrichales_60</t>
   </si>
   <si>
+    <t>Methanococci_69</t>
+  </si>
+  <si>
     <t>Sulfurovum_7</t>
   </si>
   <si>
@@ -211,6 +214,9 @@
     <t>Aquificales_14c</t>
   </si>
   <si>
+    <t>Desulfobacterales_26</t>
+  </si>
+  <si>
     <t>Thiotrichales_33</t>
   </si>
   <si>
@@ -226,9 +232,6 @@
     <t>Aquificales_21b</t>
   </si>
   <si>
-    <t>Aquificales_24</t>
-  </si>
-  <si>
     <t>Thiotrichales_27</t>
   </si>
   <si>
@@ -262,16 +265,13 @@
     <t>Candidatus Caldiarchaeum_50</t>
   </si>
   <si>
-    <t>Bin name</t>
-  </si>
-  <si>
-    <t>Desulfobacterales_26</t>
+    <t>Methanococci_24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1106,22 +1106,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1151,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1">
         <v>7.5100941463906195E-12</v>
@@ -1184,7 +1183,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1">
         <v>5.9035269128115097E-13</v>
@@ -1216,7 +1215,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1">
         <v>2.1501048792861399E-9</v>
@@ -1248,7 +1247,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1">
         <v>4.0686464032297802E-10</v>
@@ -1280,7 +1279,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1">
         <v>2.288817736608E-10</v>
@@ -1312,7 +1311,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1">
         <v>1.3038569588893999E-10</v>
@@ -1344,7 +1343,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1">
         <v>6.1396651044583305E-11</v>
@@ -1376,51 +1375,51 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.1190728358896899E-10</v>
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>2.3362094161169401E-6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.3517616279819901E-8</v>
+        <v>1.6018493794326699E-8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>2.5330067577254599E-8</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.72278367211095E-10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1.43163975726931E-10</v>
+        <v>5.1986507510307598E-10</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>1.31132182093068E-10</v>
+        <v>3.4006664207128901E-9</v>
       </c>
       <c r="I9" s="1">
-        <v>1.6018189818499999E-7</v>
+        <v>2.70821504942581E-8</v>
       </c>
       <c r="J9" s="1">
-        <v>6.7210297191799596E-7</v>
+        <v>1.13475857241608E-7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.0232116973676401E-10</v>
       </c>
       <c r="C10" s="1">
-        <v>1.6018493794326699E-8</v>
+        <v>2.46500759228683E-7</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
-        <v>5.1986507510307598E-10</v>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1429,187 +1428,187 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>3.4006664207128901E-9</v>
+        <v>1.5496047417763401E-9</v>
       </c>
       <c r="I10" s="1">
-        <v>2.70821504942581E-8</v>
+        <v>9.6809360710436895E-7</v>
       </c>
       <c r="J10" s="1">
-        <v>1.13475857241608E-7</v>
+        <v>1.0131575473411799E-5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1">
-        <v>2.0232116973676401E-10</v>
+        <v>3.4015838761865399E-9</v>
       </c>
       <c r="C11" s="1">
-        <v>2.46500759228683E-7</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
+        <v>1.0468642258411499E-6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2.0009242424506899E-7</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6.5069885462653804E-7</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.54322961673739E-6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6.4086305908049303E-7</v>
       </c>
       <c r="H11" s="1">
-        <v>1.5496047417763401E-9</v>
+        <v>1.172579591302E-8</v>
       </c>
       <c r="I11" s="1">
-        <v>9.6809360710436895E-7</v>
+        <v>8.0264590009926105E-7</v>
       </c>
       <c r="J11" s="1">
-        <v>1.0131575473411799E-5</v>
+        <v>2.8888030102024001E-6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1">
-        <v>3.4015838761865399E-9</v>
+        <v>7.0383568887471996E-11</v>
       </c>
       <c r="C12" s="1">
-        <v>1.0468642258411499E-6</v>
+        <v>4.4030065142108599E-7</v>
       </c>
       <c r="D12" s="1">
-        <v>2.0009242424506899E-7</v>
+        <v>1.55163228648283E-7</v>
       </c>
       <c r="E12" s="1">
-        <v>6.5069885462653804E-7</v>
+        <v>8.0174848971151997E-7</v>
       </c>
       <c r="F12" s="1">
-        <v>1.54322961673739E-6</v>
+        <v>5.4505169809194097E-7</v>
       </c>
       <c r="G12" s="1">
-        <v>6.4086305908049303E-7</v>
+        <v>4.3316689913207698E-7</v>
       </c>
       <c r="H12" s="1">
-        <v>1.172579591302E-8</v>
+        <v>1.28768737536869E-8</v>
       </c>
       <c r="I12" s="1">
-        <v>8.0264590009926105E-7</v>
+        <v>4.6278964223957099E-7</v>
       </c>
       <c r="J12" s="1">
-        <v>2.8888030102024001E-6</v>
+        <v>1.9457766821380498E-6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
-        <v>7.0383568887471996E-11</v>
+        <v>1.80452903038229E-8</v>
       </c>
       <c r="C13" s="1">
-        <v>4.4030065142108599E-7</v>
+        <v>1.4616043874393999E-7</v>
       </c>
       <c r="D13" s="1">
-        <v>1.55163228648283E-7</v>
+        <v>1.3427616879081601E-10</v>
       </c>
       <c r="E13" s="1">
-        <v>8.0174848971151997E-7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>5.4505169809194097E-7</v>
+        <v>3.4213256599211902E-10</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>4.3316689913207698E-7</v>
+        <v>1.64033095046195E-10</v>
       </c>
       <c r="H13" s="1">
-        <v>1.28768737536869E-8</v>
+        <v>8.7336486458827295E-7</v>
       </c>
       <c r="I13" s="1">
-        <v>4.6278964223957099E-7</v>
+        <v>6.5904464980900497E-9</v>
       </c>
       <c r="J13" s="1">
-        <v>1.9457766821380498E-6</v>
+        <v>1.7528027308660398E-11</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1.80452903038229E-8</v>
+        <v>1.31614106307274E-8</v>
       </c>
       <c r="C14" s="1">
-        <v>1.4616043874393999E-7</v>
+        <v>3.5329369797471001E-9</v>
       </c>
       <c r="D14" s="1">
-        <v>1.3427616879081601E-10</v>
+        <v>1.7336309453598901E-8</v>
       </c>
       <c r="E14" s="1">
-        <v>3.4213256599211902E-10</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
+        <v>5.0839728981610498E-10</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.3175142491703999E-9</v>
       </c>
       <c r="G14" s="1">
-        <v>1.64033095046195E-10</v>
+        <v>5.9278938217906698E-9</v>
       </c>
       <c r="H14" s="1">
-        <v>8.7336486458827295E-7</v>
+        <v>1.21621486644782E-6</v>
       </c>
       <c r="I14" s="1">
-        <v>6.5904464980900497E-9</v>
+        <v>2.03194393606219E-10</v>
       </c>
       <c r="J14" s="1">
-        <v>1.7528027308660398E-11</v>
+        <v>1.98088824324654E-11</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1">
-        <v>1.31614106307274E-8</v>
+        <v>4.4099331884926004E-12</v>
       </c>
       <c r="C15" s="1">
-        <v>3.5329369797471001E-9</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.7336309453598901E-8</v>
-      </c>
-      <c r="E15" s="1">
-        <v>5.0839728981610498E-10</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1.3175142491703999E-9</v>
-      </c>
-      <c r="G15" s="1">
-        <v>5.9278938217906698E-9</v>
+        <v>1.9478320331317199E-9</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1.21621486644782E-6</v>
+        <v>3.7911219433906001E-9</v>
       </c>
       <c r="I15" s="1">
-        <v>2.03194393606219E-10</v>
+        <v>5.6235516925483904E-9</v>
       </c>
       <c r="J15" s="1">
-        <v>1.98088824324654E-11</v>
+        <v>9.1083520638077903E-8</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1">
-        <v>4.4099331884926004E-12</v>
+        <v>1.6992959450866101E-9</v>
       </c>
       <c r="C16" s="1">
-        <v>1.9478320331317199E-9</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <v>7.1206843929104204E-11</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.27037852902711E-11</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1621,114 +1620,114 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>3.7911219433906001E-9</v>
+        <v>7.1817413038737096E-7</v>
       </c>
       <c r="I16" s="1">
-        <v>5.6235516925483904E-9</v>
+        <v>1.5422298947035101E-11</v>
       </c>
       <c r="J16" s="1">
-        <v>9.1083520638077903E-8</v>
+        <v>7.3262373736330106E-11</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1">
-        <v>1.6992959450866101E-9</v>
+        <v>1.9674996133441099E-9</v>
       </c>
       <c r="C17" s="1">
-        <v>7.1206843929104204E-11</v>
+        <v>8.1817259323050098E-10</v>
       </c>
       <c r="D17" s="1">
-        <v>1.27037852902711E-11</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
+        <v>4.9002770921656399E-9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.4213961445467E-11</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>0</v>
+      <c r="G17" s="1">
+        <v>2.9838973810856599E-10</v>
       </c>
       <c r="H17" s="1">
-        <v>7.1817413038737096E-7</v>
+        <v>2.8717687167241901E-6</v>
       </c>
       <c r="I17" s="1">
-        <v>1.5422298947035101E-11</v>
+        <v>1.43495395401035E-10</v>
       </c>
       <c r="J17" s="1">
-        <v>7.3262373736330106E-11</v>
+        <v>2.4039076923580702E-10</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1">
-        <v>1.9674996133441099E-9</v>
+        <v>1.5405066069611599E-8</v>
       </c>
       <c r="C18" s="1">
-        <v>8.1817259323050098E-10</v>
+        <v>2.8164034609969999E-8</v>
       </c>
       <c r="D18" s="1">
-        <v>4.9002770921656399E-9</v>
+        <v>4.9249554019809099E-9</v>
       </c>
       <c r="E18" s="1">
-        <v>1.4213961445467E-11</v>
+        <v>6.9726203504135396E-11</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>2.9838973810856599E-10</v>
+        <v>4.5245306142686701E-11</v>
       </c>
       <c r="H18" s="1">
-        <v>2.8717687167241901E-6</v>
+        <v>1.9653596144583699E-6</v>
       </c>
       <c r="I18" s="1">
-        <v>1.43495395401035E-10</v>
+        <v>5.1292208280289398E-9</v>
       </c>
       <c r="J18" s="1">
-        <v>2.4039076923580702E-10</v>
+        <v>7.0679671433304099E-10</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>1.5405066069611599E-8</v>
+        <v>2.9257420995971201E-8</v>
       </c>
       <c r="C19" s="1">
-        <v>2.8164034609969999E-8</v>
+        <v>8.00226484459657E-8</v>
       </c>
       <c r="D19" s="1">
-        <v>4.9249554019809099E-9</v>
+        <v>1.12329032349586E-9</v>
       </c>
       <c r="E19" s="1">
-        <v>6.9726203504135396E-11</v>
+        <v>1.8842189500042501E-9</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <v>4.5245306142686701E-11</v>
+        <v>1.0890693751870299E-9</v>
       </c>
       <c r="H19" s="1">
-        <v>1.9653596144583699E-6</v>
+        <v>1.31923288289706E-8</v>
       </c>
       <c r="I19" s="1">
-        <v>5.1292208280289398E-9</v>
+        <v>1.5606305893247301E-7</v>
       </c>
       <c r="J19" s="1">
-        <v>7.0679671433304099E-10</v>
+        <v>1.46489927350416E-11</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1">
         <v>1.48707562446063E-8</v>
@@ -1760,659 +1759,659 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1">
-        <v>2.9257420995971201E-8</v>
+        <v>2.2179627022207799E-9</v>
       </c>
       <c r="C21" s="1">
-        <v>8.00226484459657E-8</v>
+        <v>6.3299613147824599E-9</v>
       </c>
       <c r="D21" s="1">
-        <v>1.12329032349586E-9</v>
+        <v>2.1719779189915898E-8</v>
       </c>
       <c r="E21" s="1">
-        <v>1.8842189500042501E-9</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
+        <v>5.8077034326496799E-8</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.9202446167684501E-8</v>
       </c>
       <c r="G21" s="1">
-        <v>1.0890693751870299E-9</v>
+        <v>2.2033108739314501E-7</v>
       </c>
       <c r="H21" s="1">
-        <v>1.31923288289706E-8</v>
+        <v>4.7764308302495999E-10</v>
       </c>
       <c r="I21" s="1">
-        <v>1.5606305893247301E-7</v>
+        <v>1.56999448572865E-8</v>
       </c>
       <c r="J21" s="1">
-        <v>1.46489927350416E-11</v>
+        <v>7.9621461039245496E-10</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>2.2179627022207799E-9</v>
+        <v>1.2252387468494201E-7</v>
       </c>
       <c r="C22" s="1">
-        <v>6.3299613147824599E-9</v>
+        <v>2.9425793738348598E-11</v>
       </c>
       <c r="D22" s="1">
-        <v>2.1719779189915898E-8</v>
-      </c>
-      <c r="E22" s="1">
-        <v>5.8077034326496799E-8</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1.9202446167684501E-8</v>
+        <v>5.8328201321265197E-10</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>2.2033108739314501E-7</v>
+        <v>4.5851314243300901E-10</v>
       </c>
       <c r="H22" s="1">
-        <v>4.7764308302495999E-10</v>
+        <v>4.2285708776183901E-8</v>
       </c>
       <c r="I22" s="1">
-        <v>1.56999448572865E-8</v>
+        <v>4.27255070703342E-11</v>
       </c>
       <c r="J22" s="1">
-        <v>7.9621461039245496E-10</v>
+        <v>1.8433122879091899E-11</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>1.2252387468494201E-7</v>
+        <v>9.9742442593185401E-8</v>
       </c>
       <c r="C23" s="1">
-        <v>2.9425793738348598E-11</v>
+        <v>4.57554098888976E-8</v>
       </c>
       <c r="D23" s="1">
-        <v>5.8328201321265197E-10</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
+        <v>7.8460558792808494E-8</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3.3159621808421998E-8</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.5891568250015299E-8</v>
       </c>
       <c r="G23" s="1">
-        <v>4.5851314243300901E-10</v>
+        <v>2.9904631391711002E-8</v>
       </c>
       <c r="H23" s="1">
-        <v>4.2285708776183901E-8</v>
+        <v>1.8550188608992699E-8</v>
       </c>
       <c r="I23" s="1">
-        <v>4.27255070703342E-11</v>
+        <v>2.2292833655799301E-8</v>
       </c>
       <c r="J23" s="1">
-        <v>1.8433122879091899E-11</v>
+        <v>3.1816468198742902E-11</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1">
-        <v>9.9742442593185401E-8</v>
+        <v>1.1831368432357501E-8</v>
       </c>
       <c r="C24" s="1">
-        <v>4.57554098888976E-8</v>
+        <v>1.84205009085207E-7</v>
       </c>
       <c r="D24" s="1">
-        <v>7.8460558792808494E-8</v>
+        <v>6.2393968748589904E-8</v>
       </c>
       <c r="E24" s="1">
-        <v>3.3159621808421998E-8</v>
+        <v>1.44936543200113E-7</v>
       </c>
       <c r="F24" s="1">
-        <v>1.5891568250015299E-8</v>
+        <v>1.9979745907377601E-7</v>
       </c>
       <c r="G24" s="1">
-        <v>2.9904631391711002E-8</v>
+        <v>5.5362218472528804E-7</v>
       </c>
       <c r="H24" s="1">
-        <v>1.8550188608992699E-8</v>
+        <v>1.38675297834887E-8</v>
       </c>
       <c r="I24" s="1">
-        <v>2.2292833655799301E-8</v>
+        <v>1.5558522859279001E-7</v>
       </c>
       <c r="J24" s="1">
-        <v>3.1816468198742902E-11</v>
+        <v>3.8049996321508603E-10</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>1.1831368432357501E-8</v>
+        <v>2.9341273737156198E-11</v>
       </c>
       <c r="C25" s="1">
-        <v>1.84205009085207E-7</v>
+        <v>5.3506536046495204E-7</v>
       </c>
       <c r="D25" s="1">
-        <v>6.2393968748589904E-8</v>
+        <v>6.8662872351606496E-8</v>
       </c>
       <c r="E25" s="1">
-        <v>1.44936543200113E-7</v>
+        <v>1.13662290583273E-7</v>
       </c>
       <c r="F25" s="1">
-        <v>1.9979745907377601E-7</v>
+        <v>3.9821911566305502E-9</v>
       </c>
       <c r="G25" s="1">
-        <v>5.5362218472528804E-7</v>
+        <v>5.5888785434693898E-9</v>
       </c>
       <c r="H25" s="1">
-        <v>1.38675297834887E-8</v>
+        <v>3.5894549269074403E-11</v>
       </c>
       <c r="I25" s="1">
-        <v>1.5558522859279001E-7</v>
+        <v>1.7389571243269399E-7</v>
       </c>
       <c r="J25" s="1">
-        <v>3.8049996321508603E-10</v>
+        <v>1.2808994317522299E-7</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1">
-        <v>2.9341273737156198E-11</v>
+        <v>1.1459458539091699E-10</v>
       </c>
       <c r="C26" s="1">
-        <v>5.3506536046495204E-7</v>
+        <v>8.3050212920285097E-7</v>
       </c>
       <c r="D26" s="1">
-        <v>6.8662872351606496E-8</v>
+        <v>1.09004786292036E-7</v>
       </c>
       <c r="E26" s="1">
-        <v>1.13662290583273E-7</v>
+        <v>1.85774622344873E-7</v>
       </c>
       <c r="F26" s="1">
-        <v>3.9821911566305502E-9</v>
+        <v>3.7413474610538097E-8</v>
       </c>
       <c r="G26" s="1">
-        <v>5.5888785434693898E-9</v>
+        <v>5.5413571424722498E-9</v>
       </c>
       <c r="H26" s="1">
-        <v>3.5894549269074403E-11</v>
+        <v>6.7334947679299297E-10</v>
       </c>
       <c r="I26" s="1">
-        <v>1.7389571243269399E-7</v>
+        <v>1.0292487048375E-7</v>
       </c>
       <c r="J26" s="1">
-        <v>1.2808994317522299E-7</v>
+        <v>1.8352755574645399E-8</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1">
-        <v>1.1459458539091699E-10</v>
+        <v>2.1190728358896899E-10</v>
       </c>
       <c r="C27" s="1">
-        <v>8.3050212920285097E-7</v>
+        <v>2.3362094161169401E-6</v>
       </c>
       <c r="D27" s="1">
-        <v>1.09004786292036E-7</v>
+        <v>1.3517616279819901E-8</v>
       </c>
       <c r="E27" s="1">
-        <v>1.85774622344873E-7</v>
+        <v>2.5330067577254599E-8</v>
       </c>
       <c r="F27" s="1">
-        <v>3.7413474610538097E-8</v>
+        <v>2.72278367211095E-10</v>
       </c>
       <c r="G27" s="1">
-        <v>5.5413571424722498E-9</v>
+        <v>1.43163975726931E-10</v>
       </c>
       <c r="H27" s="1">
-        <v>6.7334947679299297E-10</v>
+        <v>1.31132182093068E-10</v>
       </c>
       <c r="I27" s="1">
-        <v>1.0292487048375E-7</v>
+        <v>1.6018189818499999E-7</v>
       </c>
       <c r="J27" s="1">
-        <v>1.8352755574645399E-8</v>
+        <v>6.7210297191799596E-7</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1">
-        <v>1.78639491956567E-10</v>
+        <v>8.9182649721028999E-10</v>
       </c>
       <c r="C28" s="1">
-        <v>1.11267112023438E-6</v>
+        <v>1.6264131602784E-7</v>
       </c>
       <c r="D28" s="1">
-        <v>5.9592189520536599E-7</v>
+        <v>8.8627580890027702E-7</v>
       </c>
       <c r="E28" s="1">
-        <v>2.40421112702319E-7</v>
+        <v>1.33958907039014E-6</v>
       </c>
       <c r="F28" s="1">
-        <v>4.51546737333381E-9</v>
+        <v>2.75744859938389E-7</v>
       </c>
       <c r="G28" s="1">
-        <v>9.8303836618604808E-12</v>
+        <v>8.8429775671214698E-8</v>
       </c>
       <c r="H28" s="1">
-        <v>9.8299363925514603E-11</v>
+        <v>1.21671245650145E-9</v>
       </c>
       <c r="I28" s="1">
-        <v>1.6139700869477099E-7</v>
+        <v>1.61740437786588E-7</v>
       </c>
       <c r="J28" s="1">
-        <v>8.2535178999305295E-7</v>
+        <v>3.2936641586238501E-7</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1">
-        <v>2.9603460933448402E-7</v>
+        <v>1.78639491956567E-10</v>
       </c>
       <c r="C29" s="1">
-        <v>3.14925508753961E-10</v>
+        <v>1.11267112023438E-6</v>
       </c>
       <c r="D29" s="1">
-        <v>6.1073299100717501E-10</v>
+        <v>5.9592189520536599E-7</v>
       </c>
       <c r="E29" s="1">
-        <v>2.7790119611443701E-10</v>
+        <v>2.40421112702319E-7</v>
       </c>
       <c r="F29" s="1">
-        <v>9.3641476121968793E-10</v>
+        <v>4.51546737333381E-9</v>
       </c>
       <c r="G29" s="1">
-        <v>2.8038259472863701E-9</v>
+        <v>9.8303836618604808E-12</v>
       </c>
       <c r="H29" s="1">
-        <v>1.7542432298881001E-7</v>
+        <v>9.8299363925514603E-11</v>
       </c>
       <c r="I29" s="1">
-        <v>5.6588565404980903E-10</v>
+        <v>1.6139700869477099E-7</v>
       </c>
       <c r="J29" s="1">
-        <v>7.3993479843271699E-11</v>
+        <v>8.2535178999305295E-7</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B30" s="1">
-        <v>5.2213889582653804E-7</v>
+        <v>2.9603460933448402E-7</v>
       </c>
       <c r="C30" s="1">
-        <v>1.69009279317247E-10</v>
+        <v>3.14925508753961E-10</v>
       </c>
       <c r="D30" s="1">
-        <v>1.0972706503712999E-9</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
+        <v>6.1073299100717501E-10</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2.7790119611443701E-10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>9.3641476121968793E-10</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2.8038259472863701E-9</v>
       </c>
       <c r="H30" s="1">
-        <v>1.5998751877801301E-7</v>
+        <v>1.7542432298881001E-7</v>
       </c>
       <c r="I30" s="1">
-        <v>8.733643638291E-11</v>
+        <v>5.6588565404980903E-10</v>
       </c>
       <c r="J30" s="1">
-        <v>5.2808908192406197E-11</v>
+        <v>7.3993479843271699E-11</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1">
-        <v>3.30086217628937E-8</v>
+        <v>5.2213889582653804E-7</v>
       </c>
       <c r="C31" s="1">
-        <v>6.6818629275070699E-10</v>
+        <v>1.69009279317247E-10</v>
       </c>
       <c r="D31" s="1">
-        <v>1.74024023726843E-9</v>
-      </c>
-      <c r="E31" s="1">
-        <v>9.16631984746869E-10</v>
-      </c>
-      <c r="F31" s="1">
-        <v>3.6268672728394198E-9</v>
-      </c>
-      <c r="G31" s="1">
-        <v>2.32661538816141E-8</v>
+        <v>1.0972706503712999E-9</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
       </c>
       <c r="H31" s="1">
-        <v>1.5239442508193899E-7</v>
+        <v>1.5998751877801301E-7</v>
       </c>
       <c r="I31" s="1">
-        <v>6.0356228256087097E-11</v>
+        <v>8.733643638291E-11</v>
       </c>
       <c r="J31" s="1">
-        <v>3.2809718886611103E-11</v>
+        <v>5.2808908192406197E-11</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1">
-        <v>3.11172415240962E-7</v>
+        <v>3.30086217628937E-8</v>
       </c>
       <c r="C32" s="1">
-        <v>7.6677140352572195E-11</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
+        <v>6.6818629275070699E-10</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.74024023726843E-9</v>
+      </c>
+      <c r="E32" s="1">
+        <v>9.16631984746869E-10</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3.6268672728394198E-9</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2.32661538816141E-8</v>
       </c>
       <c r="H32" s="1">
-        <v>2.8418031647757799E-8</v>
+        <v>1.5239442508193899E-7</v>
       </c>
       <c r="I32" s="1">
-        <v>3.7557958558698001E-11</v>
+        <v>6.0356228256087097E-11</v>
       </c>
       <c r="J32" s="1">
-        <v>3.4338618300342299E-11</v>
+        <v>3.2809718886611103E-11</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1">
-        <v>1.2753655335060399E-10</v>
+        <v>3.11172415240962E-7</v>
       </c>
       <c r="C33" s="1">
-        <v>7.4294665266920203E-7</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.3223331148946199E-9</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2.2848562241945101E-9</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1.5539714987940901E-10</v>
-      </c>
-      <c r="G33" s="1">
-        <v>3.0206903940873398E-9</v>
+        <v>7.6677140352572195E-11</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
       </c>
       <c r="H33" s="1">
-        <v>9.6872944233841892E-10</v>
+        <v>2.8418031647757799E-8</v>
       </c>
       <c r="I33" s="1">
-        <v>1.1288077244678E-8</v>
+        <v>3.7557958558698001E-11</v>
       </c>
       <c r="J33" s="1">
-        <v>4.3719499478300802E-9</v>
+        <v>3.4338618300342299E-11</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1">
-        <v>4.6495506157382703E-11</v>
+        <v>1.2753655335060399E-10</v>
       </c>
       <c r="C34" s="1">
-        <v>1.95563797674469E-9</v>
+        <v>7.4294665266920203E-7</v>
       </c>
       <c r="D34" s="1">
-        <v>3.17708628722708E-11</v>
+        <v>1.3223331148946199E-9</v>
       </c>
       <c r="E34" s="1">
-        <v>1.3707313796418201E-10</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
+        <v>2.2848562241945101E-9</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.5539714987940901E-10</v>
       </c>
       <c r="G34" s="1">
-        <v>5.9573529681761599E-9</v>
+        <v>3.0206903940873398E-9</v>
       </c>
       <c r="H34" s="1">
-        <v>4.17545273016907E-8</v>
+        <v>9.6872944233841892E-10</v>
       </c>
       <c r="I34" s="1">
-        <v>9.3167644524800001E-9</v>
+        <v>1.1288077244678E-8</v>
       </c>
       <c r="J34" s="1">
-        <v>1.1836261782509E-8</v>
+        <v>4.3719499478300802E-9</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1">
-        <v>1.12830372028931E-7</v>
+        <v>4.6495506157382703E-11</v>
       </c>
       <c r="C35" s="1">
-        <v>3.47282972445229E-9</v>
+        <v>1.95563797674469E-9</v>
       </c>
       <c r="D35" s="1">
-        <v>1.3292307022681999E-9</v>
+        <v>3.17708628722708E-11</v>
       </c>
       <c r="E35" s="1">
-        <v>1.38101290334298E-9</v>
+        <v>1.3707313796418201E-10</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <v>5.8565227494166799E-10</v>
+        <v>5.9573529681761599E-9</v>
       </c>
       <c r="H35" s="1">
-        <v>1.7827782723376199E-7</v>
+        <v>4.17545273016907E-8</v>
       </c>
       <c r="I35" s="1">
-        <v>1.8523235907662001E-11</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
+        <v>9.3167644524800001E-9</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1.1836261782509E-8</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1">
-        <v>6.9853217086413603E-8</v>
+        <v>1.12830372028931E-7</v>
       </c>
       <c r="C36" s="1">
-        <v>4.3911303374510201E-6</v>
+        <v>3.47282972445229E-9</v>
       </c>
       <c r="D36" s="1">
-        <v>3.7138830944760101E-6</v>
+        <v>1.3292307022681999E-9</v>
       </c>
       <c r="E36" s="1">
-        <v>9.8499273442018408E-6</v>
-      </c>
-      <c r="F36" s="1">
-        <v>5.1727651922126296E-7</v>
+        <v>1.38101290334298E-9</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
       </c>
       <c r="G36" s="1">
-        <v>1.3901946159454E-6</v>
+        <v>5.8565227494166799E-10</v>
       </c>
       <c r="H36" s="1">
-        <v>1.0352874798351E-6</v>
+        <v>1.7827782723376199E-7</v>
       </c>
       <c r="I36" s="1">
-        <v>1.1476323517811901E-6</v>
-      </c>
-      <c r="J36" s="1">
-        <v>2.0172741583438199E-7</v>
+        <v>1.8523235907662001E-11</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>5.3500891381209496E-9</v>
+        <v>6.9853217086413603E-8</v>
       </c>
       <c r="C37" s="1">
-        <v>3.2698017271523301E-8</v>
+        <v>4.3911303374510201E-6</v>
       </c>
       <c r="D37" s="1">
-        <v>6.9545573790506805E-8</v>
+        <v>3.7138830944760101E-6</v>
       </c>
       <c r="E37" s="1">
-        <v>2.0270493798798201E-7</v>
+        <v>9.8499273442018408E-6</v>
       </c>
       <c r="F37" s="1">
-        <v>3.4895126924056599E-7</v>
+        <v>5.1727651922126296E-7</v>
       </c>
       <c r="G37" s="1">
-        <v>8.6161249699967596E-7</v>
+        <v>1.3901946159454E-6</v>
       </c>
       <c r="H37" s="1">
-        <v>4.8903129497388301E-9</v>
+        <v>1.0352874798351E-6</v>
       </c>
       <c r="I37" s="1">
-        <v>3.0307643659652403E-8</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
+        <v>1.1476323517811901E-6</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2.0172741583438199E-7</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1">
-        <v>1.05658401492459E-8</v>
+        <v>5.3500891381209496E-9</v>
       </c>
       <c r="C38" s="1">
-        <v>2.1500442352986901E-8</v>
+        <v>3.2698017271523301E-8</v>
       </c>
       <c r="D38" s="1">
-        <v>6.5428116252356196E-7</v>
+        <v>6.9545573790506805E-8</v>
       </c>
       <c r="E38" s="1">
-        <v>9.2929809666666598E-7</v>
+        <v>2.0270493798798201E-7</v>
       </c>
       <c r="F38" s="1">
-        <v>2.8745887494441998E-7</v>
+        <v>3.4895126924056599E-7</v>
       </c>
       <c r="G38" s="1">
-        <v>5.9531825590648003E-7</v>
+        <v>8.6161249699967596E-7</v>
       </c>
       <c r="H38" s="1">
-        <v>1.69758619273051E-8</v>
+        <v>4.8903129497388301E-9</v>
       </c>
       <c r="I38" s="1">
-        <v>1.8381411051459399E-8</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1.98932603365405E-11</v>
+        <v>3.0307643659652403E-8</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1">
-        <v>8.4779216110208393E-8</v>
+        <v>1.05658401492459E-8</v>
       </c>
       <c r="C39" s="1">
-        <v>3.72590315191378E-7</v>
+        <v>2.1500442352986901E-8</v>
       </c>
       <c r="D39" s="1">
-        <v>7.29424736145276E-7</v>
+        <v>6.5428116252356196E-7</v>
       </c>
       <c r="E39" s="1">
-        <v>8.6517394652408197E-7</v>
+        <v>9.2929809666666598E-7</v>
       </c>
       <c r="F39" s="1">
-        <v>1.5418116099000001E-7</v>
+        <v>2.8745887494441998E-7</v>
       </c>
       <c r="G39" s="1">
-        <v>9.0325176401807998E-8</v>
+        <v>5.9531825590648003E-7</v>
       </c>
       <c r="H39" s="1">
-        <v>9.4605215881527495E-9</v>
+        <v>1.69758619273051E-8</v>
       </c>
       <c r="I39" s="1">
-        <v>1.13278245925877E-7</v>
+        <v>1.8381411051459399E-8</v>
       </c>
       <c r="J39" s="1">
-        <v>1.0112538579457401E-8</v>
+        <v>1.98932603365405E-11</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B40" s="1">
-        <v>1.04280946873499E-10</v>
+        <v>8.4779216110208393E-8</v>
       </c>
       <c r="C40" s="1">
-        <v>1.24711303512735E-10</v>
+        <v>3.72590315191378E-7</v>
       </c>
       <c r="D40" s="1">
-        <v>8.3817991281026404E-11</v>
+        <v>7.29424736145276E-7</v>
       </c>
       <c r="E40" s="1">
-        <v>2.8480658124800398E-10</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
+        <v>8.6517394652408197E-7</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1.5418116099000001E-7</v>
+      </c>
+      <c r="G40" s="1">
+        <v>9.0325176401807998E-8</v>
       </c>
       <c r="H40" s="1">
-        <v>1.2016039886206201E-7</v>
+        <v>9.4605215881527495E-9</v>
       </c>
       <c r="I40" s="1">
-        <v>6.1204967670865603E-8</v>
+        <v>1.13278245925877E-7</v>
       </c>
       <c r="J40" s="1">
-        <v>3.2528793265019698E-8</v>
+        <v>1.0112538579457401E-8</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1">
-        <v>1.87980016240078E-10</v>
+        <v>1.04280946873499E-10</v>
       </c>
       <c r="C41" s="1">
-        <v>2.3618065501601001E-10</v>
+        <v>1.24711303512735E-10</v>
       </c>
       <c r="D41" s="1">
-        <v>2.1938476855391199E-10</v>
+        <v>8.3817991281026404E-11</v>
       </c>
       <c r="E41" s="1">
-        <v>4.6463500370814002E-10</v>
+        <v>2.8480658124800398E-10</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2421,30 +2420,30 @@
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <v>1.18366051440922E-7</v>
+        <v>1.2016039886206201E-7</v>
       </c>
       <c r="I41" s="1">
-        <v>5.0544287290993002E-8</v>
+        <v>6.1204967670865603E-8</v>
       </c>
       <c r="J41" s="1">
-        <v>2.1475596642543901E-8</v>
+        <v>3.2528793265019698E-8</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1">
-        <v>8.8870720273769901E-11</v>
+        <v>1.87980016240078E-10</v>
       </c>
       <c r="C42" s="1">
-        <v>1.5485878355845698E-11</v>
+        <v>2.3618065501601001E-10</v>
       </c>
       <c r="D42" s="1">
-        <v>6.7630441012973002E-11</v>
+        <v>2.1938476855391199E-10</v>
       </c>
       <c r="E42" s="1">
-        <v>9.4211929847042604E-10</v>
+        <v>4.6463500370814002E-10</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2453,301 +2452,301 @@
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <v>1.2216723926425599E-7</v>
+        <v>1.18366051440922E-7</v>
       </c>
       <c r="I42" s="1">
-        <v>6.6246740788008297E-8</v>
+        <v>5.0544287290993002E-8</v>
       </c>
       <c r="J42" s="1">
-        <v>3.1653644776579102E-8</v>
+        <v>2.1475596642543901E-8</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B43" s="1">
-        <v>5.8157817136534002E-11</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
+        <v>8.8870720273769901E-11</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1.5485878355845698E-11</v>
       </c>
       <c r="D43" s="1">
-        <v>5.3488845760109998E-10</v>
+        <v>6.7630441012973002E-11</v>
       </c>
       <c r="E43" s="1">
-        <v>1.2875862517403201E-10</v>
+        <v>9.4211929847042604E-10</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
-      <c r="G43" s="1">
-        <v>9.3433396872024501E-10</v>
+      <c r="G43">
+        <v>0</v>
       </c>
       <c r="H43" s="1">
-        <v>5.4915400079024504E-9</v>
+        <v>1.2216723926425599E-7</v>
       </c>
       <c r="I43" s="1">
-        <v>2.4734462503807799E-8</v>
+        <v>6.6246740788008297E-8</v>
       </c>
       <c r="J43" s="1">
-        <v>6.8583075360069401E-9</v>
+        <v>3.1653644776579102E-8</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B44" s="1">
-        <v>9.389017430542749E-10</v>
-      </c>
-      <c r="C44" s="1">
-        <v>3.48984983753936E-10</v>
+        <v>5.8157817136534002E-11</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
       </c>
       <c r="D44" s="1">
-        <v>2.8262365654969098E-10</v>
+        <v>5.3488845760109998E-10</v>
       </c>
       <c r="E44" s="1">
-        <v>7.6187291319614495E-12</v>
+        <v>1.2875862517403201E-10</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>4.0266766164101E-10</v>
+        <v>9.3433396872024501E-10</v>
       </c>
       <c r="H44" s="1">
-        <v>4.5376974639924797E-8</v>
+        <v>5.4915400079024504E-9</v>
       </c>
       <c r="I44" s="1">
-        <v>1.7854034487783901E-8</v>
+        <v>2.4734462503807799E-8</v>
       </c>
       <c r="J44" s="1">
-        <v>7.0956288409717499E-9</v>
+        <v>6.8583075360069401E-9</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B45" s="1">
-        <v>8.6840178067093402E-11</v>
+        <v>9.389017430542749E-10</v>
       </c>
       <c r="C45" s="1">
-        <v>5.8333045121591906E-11</v>
+        <v>3.48984983753936E-10</v>
       </c>
       <c r="D45" s="1">
-        <v>2.47636355693181E-10</v>
+        <v>2.8262365654969098E-10</v>
       </c>
       <c r="E45" s="1">
-        <v>1.1638553619040501E-11</v>
+        <v>7.6187291319614495E-12</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45" s="1">
-        <v>5.3766369814434998E-10</v>
+        <v>4.0266766164101E-10</v>
       </c>
       <c r="H45" s="1">
-        <v>4.5168597172769601E-8</v>
+        <v>4.5376974639924797E-8</v>
       </c>
       <c r="I45" s="1">
-        <v>1.8898057301937401E-8</v>
+        <v>1.7854034487783901E-8</v>
       </c>
       <c r="J45" s="1">
-        <v>6.6581283897606599E-9</v>
+        <v>7.0956288409717499E-9</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1">
-        <v>4.7120057675604097E-11</v>
+        <v>8.6840178067093402E-11</v>
       </c>
       <c r="C46" s="1">
-        <v>3.0586543334144897E-11</v>
+        <v>5.8333045121591906E-11</v>
       </c>
       <c r="D46" s="1">
-        <v>1.5821038079947099E-10</v>
+        <v>2.47636355693181E-10</v>
       </c>
       <c r="E46" s="1">
-        <v>2.5243125559307001E-11</v>
+        <v>1.1638553619040501E-11</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46" s="1">
-        <v>2.6914499718520101E-10</v>
+        <v>5.3766369814434998E-10</v>
       </c>
       <c r="H46" s="1">
-        <v>4.37441628838767E-8</v>
+        <v>4.5168597172769601E-8</v>
       </c>
       <c r="I46" s="1">
-        <v>1.9114594105509599E-8</v>
+        <v>1.8898057301937401E-8</v>
       </c>
       <c r="J46" s="1">
-        <v>8.3189737462623503E-9</v>
+        <v>6.6581283897606599E-9</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B47" s="1">
-        <v>1.8762247992749301E-8</v>
+        <v>4.7120057675604097E-11</v>
       </c>
       <c r="C47" s="1">
-        <v>1.42189996661214E-8</v>
+        <v>3.0586543334144897E-11</v>
       </c>
       <c r="D47" s="1">
-        <v>1.2882598221378101E-6</v>
+        <v>1.5821038079947099E-10</v>
       </c>
       <c r="E47" s="1">
-        <v>8.3826242776269203E-7</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1.3269571898838E-7</v>
+        <v>2.5243125559307001E-11</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
       </c>
       <c r="G47" s="1">
-        <v>8.7727511338976495E-7</v>
+        <v>2.6914499718520101E-10</v>
       </c>
       <c r="H47" s="1">
-        <v>2.9323051711819199E-8</v>
+        <v>4.37441628838767E-8</v>
       </c>
       <c r="I47" s="1">
-        <v>3.2418424527106303E-8</v>
+        <v>1.9114594105509599E-8</v>
       </c>
       <c r="J47" s="1">
-        <v>2.3634052122613099E-12</v>
+        <v>8.3189737462623503E-9</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B48" s="1">
-        <v>1.9342036093501101E-7</v>
+        <v>1.8762247992749301E-8</v>
       </c>
       <c r="C48" s="1">
-        <v>1.0255856257012701E-5</v>
+        <v>1.42189996661214E-8</v>
       </c>
       <c r="D48" s="1">
-        <v>2.0271811398251501E-7</v>
+        <v>1.2882598221378101E-6</v>
       </c>
       <c r="E48" s="1">
-        <v>1.5402803328073199E-7</v>
+        <v>8.3826242776269203E-7</v>
       </c>
       <c r="F48" s="1">
-        <v>1.5321785285931999E-7</v>
+        <v>1.3269571898838E-7</v>
       </c>
       <c r="G48" s="1">
-        <v>2.6203950507658002E-7</v>
+        <v>8.7727511338976495E-7</v>
       </c>
       <c r="H48" s="1">
-        <v>4.12619491874833E-7</v>
+        <v>2.9323051711819199E-8</v>
       </c>
       <c r="I48" s="1">
-        <v>8.4595546151278898E-6</v>
+        <v>3.2418424527106303E-8</v>
       </c>
       <c r="J48" s="1">
-        <v>2.2004758153962399E-8</v>
+        <v>2.3634052122613099E-12</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B49" s="1">
-        <v>2.07074911436416E-8</v>
+        <v>1.9342036093501101E-7</v>
       </c>
       <c r="C49" s="1">
-        <v>5.5416083555822705E-7</v>
+        <v>1.0255856257012701E-5</v>
       </c>
       <c r="D49" s="1">
-        <v>4.1041908173055803E-6</v>
+        <v>2.0271811398251501E-7</v>
       </c>
       <c r="E49" s="1">
-        <v>6.4445816814579196E-6</v>
+        <v>1.5402803328073199E-7</v>
       </c>
       <c r="F49" s="1">
-        <v>8.6140010289177593E-6</v>
+        <v>1.5321785285931999E-7</v>
       </c>
       <c r="G49" s="1">
-        <v>9.6962397202923396E-6</v>
+        <v>2.6203950507658002E-7</v>
       </c>
       <c r="H49" s="1">
-        <v>1.9345622959398801E-8</v>
+        <v>4.12619491874833E-7</v>
       </c>
       <c r="I49" s="1">
-        <v>3.3648755110841601E-7</v>
+        <v>8.4595546151278898E-6</v>
       </c>
       <c r="J49" s="1">
-        <v>6.1519749329859196E-10</v>
+        <v>2.2004758153962399E-8</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B50" s="1">
-        <v>1.81282238175605E-7</v>
+        <v>2.07074911436416E-8</v>
       </c>
       <c r="C50" s="1">
-        <v>8.4269254539393899E-9</v>
+        <v>5.5416083555822705E-7</v>
       </c>
       <c r="D50" s="1">
-        <v>2.3742634708455002E-9</v>
+        <v>4.1041908173055803E-6</v>
       </c>
       <c r="E50" s="1">
-        <v>6.2355771769855404E-9</v>
+        <v>6.4445816814579196E-6</v>
       </c>
       <c r="F50" s="1">
-        <v>1.6209681473214499E-8</v>
+        <v>8.6140010289177593E-6</v>
       </c>
       <c r="G50" s="1">
-        <v>7.2111261497494105E-8</v>
+        <v>9.6962397202923396E-6</v>
       </c>
       <c r="H50" s="1">
-        <v>9.0336362739818798E-8</v>
+        <v>1.9345622959398801E-8</v>
       </c>
       <c r="I50" s="1">
-        <v>9.2856773038353595E-9</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
+        <v>3.3648755110841601E-7</v>
+      </c>
+      <c r="J50" s="1">
+        <v>6.1519749329859196E-10</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B51" s="1">
-        <v>2.5192705636997401E-8</v>
+        <v>1.81282238175605E-7</v>
       </c>
       <c r="C51" s="1">
-        <v>5.1311229712752701E-8</v>
+        <v>8.4269254539393899E-9</v>
       </c>
       <c r="D51" s="1">
-        <v>4.8679849721639997E-7</v>
+        <v>2.3742634708455002E-9</v>
       </c>
       <c r="E51" s="1">
-        <v>4.1521741485987902E-7</v>
+        <v>6.2355771769855404E-9</v>
       </c>
       <c r="F51" s="1">
-        <v>4.0803671077091801E-7</v>
+        <v>1.6209681473214499E-8</v>
       </c>
       <c r="G51" s="1">
-        <v>4.0748624538049402E-7</v>
+        <v>7.2111261497494105E-8</v>
       </c>
       <c r="H51" s="1">
-        <v>1.20902918731027E-8</v>
+        <v>9.0336362739818798E-8</v>
       </c>
       <c r="I51" s="1">
-        <v>4.9306715641517301E-8</v>
-      </c>
-      <c r="J51" s="1">
-        <v>4.84931836909525E-8</v>
+        <v>9.2856773038353595E-9</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -2755,95 +2754,95 @@
         <v>77</v>
       </c>
       <c r="B52" s="1">
-        <v>1.57658623084668E-8</v>
+        <v>2.5192705636997401E-8</v>
       </c>
       <c r="C52" s="1">
-        <v>5.0069411521217798E-8</v>
+        <v>5.1311229712752701E-8</v>
       </c>
       <c r="D52" s="1">
-        <v>5.4692433544470098E-8</v>
+        <v>4.8679849721639997E-7</v>
       </c>
       <c r="E52" s="1">
-        <v>6.3436976929788801E-8</v>
+        <v>4.1521741485987902E-7</v>
       </c>
       <c r="F52" s="1">
-        <v>9.1760764901082505E-8</v>
+        <v>4.0803671077091801E-7</v>
       </c>
       <c r="G52" s="1">
-        <v>2.10028020519655E-7</v>
+        <v>4.0748624538049402E-7</v>
       </c>
       <c r="H52" s="1">
-        <v>2.9962698224499498E-9</v>
+        <v>1.20902918731027E-8</v>
       </c>
       <c r="I52" s="1">
-        <v>1.0034478895889301E-7</v>
+        <v>4.9306715641517301E-8</v>
       </c>
       <c r="J52" s="1">
-        <v>1.65752622468087E-7</v>
+        <v>4.84931836909525E-8</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B53" s="1">
-        <v>3.0751703339051901E-8</v>
+        <v>1.57658623084668E-8</v>
       </c>
       <c r="C53" s="1">
-        <v>8.6467109878690606E-8</v>
+        <v>5.0069411521217798E-8</v>
       </c>
       <c r="D53" s="1">
-        <v>3.5900720122934797E-8</v>
+        <v>5.4692433544470098E-8</v>
       </c>
       <c r="E53" s="1">
-        <v>4.3565694592680702E-8</v>
+        <v>6.3436976929788801E-8</v>
       </c>
       <c r="F53" s="1">
-        <v>2.5315199856045801E-8</v>
+        <v>9.1760764901082505E-8</v>
       </c>
       <c r="G53" s="1">
-        <v>1.58911618249139E-7</v>
+        <v>2.10028020519655E-7</v>
       </c>
       <c r="H53" s="1">
-        <v>2.6752469286022E-8</v>
+        <v>2.9962698224499498E-9</v>
       </c>
       <c r="I53" s="1">
-        <v>3.5764093385885402E-8</v>
-      </c>
-      <c r="J53">
-        <v>0</v>
+        <v>1.0034478895889301E-7</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1.65752622468087E-7</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B54" s="1">
-        <v>1.6494168130828999E-8</v>
+        <v>3.0751703339051901E-8</v>
       </c>
       <c r="C54" s="1">
-        <v>2.7421200470614102E-8</v>
+        <v>8.6467109878690606E-8</v>
       </c>
       <c r="D54" s="1">
-        <v>3.6351605704833499E-7</v>
+        <v>3.5900720122934797E-8</v>
       </c>
       <c r="E54" s="1">
-        <v>2.76158480170627E-7</v>
+        <v>4.3565694592680702E-8</v>
       </c>
       <c r="F54" s="1">
-        <v>2.43152193995635E-7</v>
+        <v>2.5315199856045801E-8</v>
       </c>
       <c r="G54" s="1">
-        <v>1.0284237389691601E-7</v>
+        <v>1.58911618249139E-7</v>
       </c>
       <c r="H54" s="1">
-        <v>6.2424428674008099E-9</v>
+        <v>2.6752469286022E-8</v>
       </c>
       <c r="I54" s="1">
-        <v>4.6206521661316799E-8</v>
-      </c>
-      <c r="J54" s="1">
-        <v>5.6520340283715097E-8</v>
+        <v>3.5764093385885402E-8</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -2851,612 +2850,644 @@
         <v>39</v>
       </c>
       <c r="B55" s="1">
-        <v>2.0941907238565301E-8</v>
+        <v>1.6494168130828999E-8</v>
       </c>
       <c r="C55" s="1">
-        <v>4.6084556313681498E-7</v>
+        <v>2.7421200470614102E-8</v>
       </c>
       <c r="D55" s="1">
-        <v>5.4706650499239297E-6</v>
+        <v>3.6351605704833499E-7</v>
       </c>
       <c r="E55" s="1">
-        <v>8.33573976808801E-6</v>
+        <v>2.76158480170627E-7</v>
       </c>
       <c r="F55" s="1">
-        <v>8.7205588660453498E-6</v>
+        <v>2.43152193995635E-7</v>
       </c>
       <c r="G55" s="1">
-        <v>1.1396603682865501E-5</v>
+        <v>1.0284237389691601E-7</v>
       </c>
       <c r="H55" s="1">
-        <v>1.7018642724503699E-8</v>
+        <v>6.2424428674008099E-9</v>
       </c>
       <c r="I55" s="1">
-        <v>3.3678535289215102E-7</v>
+        <v>4.6206521661316799E-8</v>
       </c>
       <c r="J55" s="1">
-        <v>1.3046153943589399E-10</v>
+        <v>5.6520340283715097E-8</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B56" s="1">
-        <v>1.9518256346882099E-11</v>
+        <v>2.0941907238565301E-8</v>
       </c>
       <c r="C56" s="1">
-        <v>1.51340183362797E-7</v>
+        <v>4.6084556313681498E-7</v>
       </c>
       <c r="D56" s="1">
-        <v>5.6900516844296898E-8</v>
+        <v>5.4706650499239297E-6</v>
       </c>
       <c r="E56" s="1">
-        <v>3.4722569521564399E-8</v>
+        <v>8.33573976808801E-6</v>
       </c>
       <c r="F56" s="1">
-        <v>4.1428809056078002E-9</v>
+        <v>8.7205588660453498E-6</v>
       </c>
       <c r="G56" s="1">
-        <v>5.6206254565127504E-9</v>
+        <v>1.1396603682865501E-5</v>
       </c>
       <c r="H56" s="1">
-        <v>1.4211685974872099E-9</v>
+        <v>1.7018642724503699E-8</v>
       </c>
       <c r="I56" s="1">
-        <v>1.9292553846253001E-8</v>
+        <v>3.3678535289215102E-7</v>
       </c>
       <c r="J56" s="1">
-        <v>9.9359795514771696E-8</v>
+        <v>1.3046153943589399E-10</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1">
-        <v>2.3107640604494799E-9</v>
+        <v>1.9518256346882099E-11</v>
       </c>
       <c r="C57" s="1">
-        <v>9.2801577659505494E-9</v>
+        <v>1.51340183362797E-7</v>
       </c>
       <c r="D57" s="1">
-        <v>8.73489994102456E-11</v>
+        <v>5.6900516844296898E-8</v>
       </c>
       <c r="E57" s="1">
-        <v>7.7632168170575995E-11</v>
+        <v>3.4722569521564399E-8</v>
       </c>
       <c r="F57" s="1">
-        <v>1.85612429196616E-9</v>
+        <v>4.1428809056078002E-9</v>
       </c>
       <c r="G57" s="1">
-        <v>1.3608046573509299E-8</v>
+        <v>5.6206254565127504E-9</v>
       </c>
       <c r="H57" s="1">
-        <v>3.48594522140253E-8</v>
+        <v>1.4211685974872099E-9</v>
       </c>
       <c r="I57" s="1">
-        <v>8.1698592914367793E-9</v>
+        <v>1.9292553846253001E-8</v>
       </c>
       <c r="J57" s="1">
-        <v>3.7510418706446499E-8</v>
+        <v>9.9359795514771696E-8</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B58" s="1">
-        <v>7.4955666131075304E-10</v>
+        <v>2.3107640604494799E-9</v>
       </c>
       <c r="C58" s="1">
-        <v>1.2550596452246899E-7</v>
+        <v>9.2801577659505494E-9</v>
       </c>
       <c r="D58" s="1">
-        <v>9.5101239040252795E-9</v>
+        <v>8.73489994102456E-11</v>
       </c>
       <c r="E58" s="1">
-        <v>1.73906791321887E-8</v>
+        <v>7.7632168170575995E-11</v>
       </c>
       <c r="F58" s="1">
-        <v>1.9265082327130002E-9</v>
+        <v>1.85612429196616E-9</v>
       </c>
       <c r="G58" s="1">
-        <v>1.5564973354944E-9</v>
+        <v>1.3608046573509299E-8</v>
       </c>
       <c r="H58" s="1">
-        <v>8.4724805480714498E-10</v>
+        <v>3.48594522140253E-8</v>
       </c>
       <c r="I58" s="1">
-        <v>6.97948169556072E-7</v>
+        <v>8.1698592914367793E-9</v>
       </c>
       <c r="J58" s="1">
-        <v>1.6704921994673701E-5</v>
+        <v>3.7510418706446499E-8</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59" s="1">
-        <v>1.12487549975614E-10</v>
+        <v>7.4955666131075304E-10</v>
       </c>
       <c r="C59" s="1">
-        <v>5.8284197601641504E-7</v>
+        <v>1.2550596452246899E-7</v>
       </c>
       <c r="D59" s="1">
-        <v>6.0582401936176696E-9</v>
+        <v>9.5101239040252795E-9</v>
       </c>
       <c r="E59" s="1">
-        <v>9.9300616647836507E-9</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
+        <v>1.73906791321887E-8</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1.9265082327130002E-9</v>
       </c>
       <c r="G59" s="1">
-        <v>6.9420527785735502E-9</v>
+        <v>1.5564973354944E-9</v>
       </c>
       <c r="H59" s="1">
-        <v>7.8460179224159005E-10</v>
+        <v>8.4724805480714498E-10</v>
       </c>
       <c r="I59" s="1">
-        <v>3.1174009423973302E-7</v>
+        <v>6.97948169556072E-7</v>
       </c>
       <c r="J59" s="1">
-        <v>4.1122239311778903E-6</v>
+        <v>1.6704921994673701E-5</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B60" s="1">
-        <v>2.5928262361610498E-10</v>
+        <v>1.12487549975614E-10</v>
       </c>
       <c r="C60" s="1">
-        <v>4.3642396816052898E-7</v>
+        <v>5.8284197601641504E-7</v>
       </c>
       <c r="D60" s="1">
-        <v>5.0670722179276005E-7</v>
+        <v>6.0582401936176696E-9</v>
       </c>
       <c r="E60" s="1">
-        <v>8.7705041683370598E-8</v>
-      </c>
-      <c r="F60" s="1">
-        <v>3.1433457684555602E-9</v>
+        <v>9.9300616647836507E-9</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
       </c>
       <c r="G60" s="1">
-        <v>1.9624311825934098E-8</v>
+        <v>6.9420527785735502E-9</v>
       </c>
       <c r="H60" s="1">
-        <v>4.2750381976750298E-10</v>
+        <v>7.8460179224159005E-10</v>
       </c>
       <c r="I60" s="1">
-        <v>7.98186335613621E-8</v>
+        <v>3.1174009423973302E-7</v>
       </c>
       <c r="J60" s="1">
-        <v>7.09638609025978E-7</v>
+        <v>4.1122239311778903E-6</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B61" s="1">
-        <v>3.3831135268925098E-10</v>
+        <v>2.5928262361610498E-10</v>
       </c>
       <c r="C61" s="1">
-        <v>6.7681382934189797E-7</v>
+        <v>4.3642396816052898E-7</v>
       </c>
       <c r="D61" s="1">
-        <v>1.2691176662105501E-8</v>
+        <v>5.0670722179276005E-7</v>
       </c>
       <c r="E61" s="1">
-        <v>2.1031684322646799E-8</v>
+        <v>8.7705041683370598E-8</v>
       </c>
       <c r="F61" s="1">
-        <v>4.6481918335349497E-9</v>
+        <v>3.1433457684555602E-9</v>
       </c>
       <c r="G61" s="1">
-        <v>5.9305497372165803E-9</v>
+        <v>1.9624311825934098E-8</v>
       </c>
       <c r="H61" s="1">
-        <v>6.2484827310542101E-10</v>
+        <v>4.2750381976750298E-10</v>
       </c>
       <c r="I61" s="1">
-        <v>3.9675080963725902E-7</v>
+        <v>7.98186335613621E-8</v>
       </c>
       <c r="J61" s="1">
-        <v>4.3300036782881598E-6</v>
+        <v>7.09638609025978E-7</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B62" s="1">
-        <v>2.2799080930357901E-11</v>
+        <v>3.3831135268925098E-10</v>
       </c>
       <c r="C62" s="1">
-        <v>4.9636613372875698E-8</v>
+        <v>6.7681382934189797E-7</v>
       </c>
       <c r="D62" s="1">
-        <v>3.5562333480952599E-7</v>
+        <v>1.2691176662105501E-8</v>
       </c>
       <c r="E62" s="1">
-        <v>4.7212155048755202E-8</v>
+        <v>2.1031684322646799E-8</v>
       </c>
       <c r="F62" s="1">
-        <v>3.2079613423858099E-10</v>
+        <v>4.6481918335349497E-9</v>
       </c>
       <c r="G62" s="1">
-        <v>6.2917280843847498E-8</v>
+        <v>5.9305497372165803E-9</v>
       </c>
       <c r="H62" s="1">
-        <v>2.8250850427890198E-9</v>
+        <v>6.2484827310542101E-10</v>
       </c>
       <c r="I62" s="1">
-        <v>1.52165635063785E-8</v>
+        <v>3.9675080963725902E-7</v>
       </c>
       <c r="J62" s="1">
-        <v>4.34471058086015E-7</v>
+        <v>4.3300036782881598E-6</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B63" s="1">
-        <v>7.6842802665345297E-10</v>
+        <v>2.2799080930357901E-11</v>
       </c>
       <c r="C63" s="1">
-        <v>1.9904201220012499E-7</v>
+        <v>4.9636613372875698E-8</v>
       </c>
       <c r="D63" s="1">
-        <v>8.4470304180542799E-9</v>
+        <v>3.5562333480952599E-7</v>
       </c>
       <c r="E63" s="1">
-        <v>2.93852029924511E-8</v>
+        <v>4.7212155048755202E-8</v>
       </c>
       <c r="F63" s="1">
-        <v>8.2967398936837493E-9</v>
+        <v>3.2079613423858099E-10</v>
       </c>
       <c r="G63" s="1">
-        <v>2.9005595455332202E-9</v>
+        <v>6.2917280843847498E-8</v>
       </c>
       <c r="H63" s="1">
-        <v>8.5511272491389298E-10</v>
+        <v>2.8250850427890198E-9</v>
       </c>
       <c r="I63" s="1">
-        <v>1.03541102896883E-6</v>
+        <v>1.52165635063785E-8</v>
       </c>
       <c r="J63" s="1">
-        <v>2.0106418726902402E-5</v>
+        <v>4.34471058086015E-7</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B64" s="1">
-        <v>3.06423958954029E-9</v>
+        <v>7.6842802665345297E-10</v>
       </c>
       <c r="C64" s="1">
-        <v>1.1590525936140699E-8</v>
+        <v>1.9904201220012499E-7</v>
       </c>
       <c r="D64" s="1">
-        <v>9.0561921349497608E-9</v>
+        <v>8.4470304180542799E-9</v>
       </c>
       <c r="E64" s="1">
-        <v>9.1144162557095407E-9</v>
+        <v>2.93852029924511E-8</v>
       </c>
       <c r="F64" s="1">
-        <v>1.5657888732164402E-8</v>
+        <v>8.2967398936837493E-9</v>
       </c>
       <c r="G64" s="1">
-        <v>4.9623793824615703E-8</v>
+        <v>2.9005595455332202E-9</v>
       </c>
       <c r="H64" s="1">
-        <v>2.86981504128125E-9</v>
+        <v>8.5511272491389298E-10</v>
       </c>
       <c r="I64" s="1">
-        <v>5.1463791756406496E-9</v>
+        <v>1.03541102896883E-6</v>
       </c>
       <c r="J64" s="1">
-        <v>7.2196570632387101E-12</v>
+        <v>2.0106418726902402E-5</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B65" s="1">
-        <v>5.3675810577214102E-9</v>
+        <v>3.06423958954029E-9</v>
       </c>
       <c r="C65" s="1">
-        <v>8.3938960517303093E-8</v>
+        <v>1.1590525936140699E-8</v>
       </c>
       <c r="D65" s="1">
-        <v>4.65560105032354E-9</v>
+        <v>9.0561921349497608E-9</v>
       </c>
       <c r="E65" s="1">
-        <v>1.77756915158706E-9</v>
+        <v>9.1144162557095407E-9</v>
       </c>
       <c r="F65" s="1">
-        <v>2.2075553405866602E-9</v>
+        <v>1.5657888732164402E-8</v>
       </c>
       <c r="G65" s="1">
-        <v>9.1837704126426907E-9</v>
+        <v>4.9623793824615703E-8</v>
       </c>
       <c r="H65" s="1">
-        <v>5.4694151870403902E-9</v>
+        <v>2.86981504128125E-9</v>
       </c>
       <c r="I65" s="1">
-        <v>9.5296691504505106E-8</v>
+        <v>5.1463791756406496E-9</v>
       </c>
       <c r="J65" s="1">
-        <v>3.7952439838181599E-10</v>
+        <v>7.2196570632387101E-12</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="B66" s="1">
-        <v>7.3551269934524401E-8</v>
+        <v>5.3675810577214102E-9</v>
       </c>
       <c r="C66" s="1">
-        <v>3.6560354239956002E-8</v>
+        <v>8.3938960517303093E-8</v>
       </c>
       <c r="D66" s="1">
-        <v>1.33521397308002E-8</v>
+        <v>4.65560105032354E-9</v>
       </c>
       <c r="E66" s="1">
-        <v>9.6571481569315007E-9</v>
+        <v>1.77756915158706E-9</v>
       </c>
       <c r="F66" s="1">
-        <v>4.1796592988044302E-9</v>
+        <v>2.2075553405866602E-9</v>
       </c>
       <c r="G66" s="1">
-        <v>2.0856710964106E-10</v>
+        <v>9.1837704126426907E-9</v>
       </c>
       <c r="H66" s="1">
-        <v>4.9867985839053803E-8</v>
+        <v>5.4694151870403902E-9</v>
       </c>
       <c r="I66" s="1">
-        <v>2.0068868938999701E-7</v>
+        <v>9.5296691504505106E-8</v>
       </c>
       <c r="J66" s="1">
-        <v>3.5122243188501599E-7</v>
+        <v>3.7952439838181599E-10</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B67" s="1">
-        <v>3.1034325880650698E-8</v>
+        <v>7.3551269934524401E-8</v>
       </c>
       <c r="C67" s="1">
-        <v>9.6445262644122706E-9</v>
+        <v>3.6560354239956002E-8</v>
       </c>
       <c r="D67" s="1">
-        <v>1.57886003139107E-9</v>
+        <v>1.33521397308002E-8</v>
       </c>
       <c r="E67" s="1">
-        <v>4.1784904233879499E-12</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
+        <v>9.6571481569315007E-9</v>
+      </c>
+      <c r="F67" s="1">
+        <v>4.1796592988044302E-9</v>
+      </c>
+      <c r="G67" s="1">
+        <v>2.0856710964106E-10</v>
       </c>
       <c r="H67" s="1">
-        <v>2.28017635770991E-8</v>
+        <v>4.9867985839053803E-8</v>
       </c>
       <c r="I67" s="1">
-        <v>1.5866665423806799E-8</v>
+        <v>2.0068868938999701E-7</v>
       </c>
       <c r="J67" s="1">
-        <v>6.4964998607356597E-12</v>
+        <v>3.5122243188501599E-7</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="B68" s="1">
-        <v>1.2683881122589E-8</v>
+        <v>3.1034325880650698E-8</v>
       </c>
       <c r="C68" s="1">
-        <v>7.5848542546567107E-8</v>
+        <v>9.6445262644122706E-9</v>
       </c>
       <c r="D68" s="1">
-        <v>1.01416432128205E-8</v>
+        <v>1.57886003139107E-9</v>
       </c>
       <c r="E68" s="1">
-        <v>9.1611204431548799E-9</v>
-      </c>
-      <c r="F68" s="1">
-        <v>1.27189551681966E-8</v>
-      </c>
-      <c r="G68" s="1">
-        <v>4.2349969372103002E-8</v>
+        <v>4.1784904233879499E-12</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
       </c>
       <c r="H68" s="1">
-        <v>1.37503810050397E-8</v>
+        <v>2.28017635770991E-8</v>
       </c>
       <c r="I68" s="1">
-        <v>1.26034330026371E-7</v>
+        <v>1.5866665423806799E-8</v>
       </c>
       <c r="J68" s="1">
-        <v>1.36717995206376E-11</v>
+        <v>6.4964998607356597E-12</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B69" s="1">
-        <v>1.09053183137583E-8</v>
+        <v>1.2683881122589E-8</v>
       </c>
       <c r="C69" s="1">
-        <v>1.57729766997571E-7</v>
+        <v>7.5848542546567107E-8</v>
       </c>
       <c r="D69" s="1">
-        <v>5.7551390585433304E-9</v>
+        <v>1.01416432128205E-8</v>
       </c>
       <c r="E69" s="1">
-        <v>8.1687931894146198E-9</v>
+        <v>9.1611204431548799E-9</v>
       </c>
       <c r="F69" s="1">
-        <v>1.14959605930169E-8</v>
+        <v>1.27189551681966E-8</v>
       </c>
       <c r="G69" s="1">
-        <v>2.9321194286304701E-8</v>
+        <v>4.2349969372103002E-8</v>
       </c>
       <c r="H69" s="1">
-        <v>1.6524780217957602E-8</v>
+        <v>1.37503810050397E-8</v>
       </c>
       <c r="I69" s="1">
-        <v>1.3728304238166401E-7</v>
+        <v>1.26034330026371E-7</v>
       </c>
       <c r="J69" s="1">
-        <v>3.89329809471127E-10</v>
+        <v>1.36717995206376E-11</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B70" s="1">
-        <v>6.8327299338592398E-10</v>
+        <v>1.09053183137583E-8</v>
       </c>
       <c r="C70" s="1">
-        <v>6.9385680728382995E-8</v>
+        <v>1.57729766997571E-7</v>
       </c>
       <c r="D70" s="1">
-        <v>5.9863833971336401E-9</v>
+        <v>5.7551390585433304E-9</v>
       </c>
       <c r="E70" s="1">
-        <v>2.6212524702360301E-8</v>
+        <v>8.1687931894146198E-9</v>
       </c>
       <c r="F70" s="1">
-        <v>1.03158895379353E-7</v>
+        <v>1.14959605930169E-8</v>
       </c>
       <c r="G70" s="1">
-        <v>5.7856305898109299E-8</v>
+        <v>2.9321194286304701E-8</v>
       </c>
       <c r="H70" s="1">
-        <v>6.4205763923349803E-9</v>
+        <v>1.6524780217957602E-8</v>
       </c>
       <c r="I70" s="1">
-        <v>6.2269595671175396E-8</v>
+        <v>1.3728304238166401E-7</v>
       </c>
       <c r="J70" s="1">
-        <v>3.6305293470062397E-11</v>
+        <v>3.89329809471127E-10</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B71" s="1">
-        <v>1.6257529984080401E-7</v>
+        <v>6.8327299338592398E-10</v>
       </c>
       <c r="C71" s="1">
-        <v>1.6253875114748699E-8</v>
+        <v>6.9385680728382995E-8</v>
       </c>
       <c r="D71" s="1">
-        <v>3.6140670636490897E-8</v>
+        <v>5.9863833971336401E-9</v>
       </c>
       <c r="E71" s="1">
-        <v>4.86244936945541E-8</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
+        <v>2.6212524702360301E-8</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1.03158895379353E-7</v>
       </c>
       <c r="G71" s="1">
-        <v>1.0084468504467799E-8</v>
+        <v>5.7856305898109299E-8</v>
       </c>
       <c r="H71" s="1">
-        <v>5.0924440747513698E-8</v>
+        <v>6.4205763923349803E-9</v>
       </c>
       <c r="I71" s="1">
-        <v>6.2873727870719703E-9</v>
+        <v>6.2269595671175396E-8</v>
       </c>
       <c r="J71" s="1">
-        <v>4.8878481302112298E-11</v>
+        <v>3.6305293470062397E-11</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1">
-        <v>2.8113596911919501E-9</v>
+        <v>1.6257529984080401E-7</v>
       </c>
       <c r="C72" s="1">
-        <v>8.7211024432964898E-9</v>
+        <v>1.6253875114748699E-8</v>
       </c>
       <c r="D72" s="1">
-        <v>6.62989507356424E-9</v>
+        <v>3.6140670636490897E-8</v>
       </c>
       <c r="E72" s="1">
-        <v>9.1813788006872907E-9</v>
-      </c>
-      <c r="F72" s="1">
-        <v>1.52400261368346E-8</v>
+        <v>4.86244936945541E-8</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
       </c>
       <c r="G72" s="1">
-        <v>7.5360529725183904E-8</v>
+        <v>1.0084468504467799E-8</v>
       </c>
       <c r="H72" s="1">
-        <v>2.8566357397374601E-9</v>
+        <v>5.0924440747513698E-8</v>
       </c>
       <c r="I72" s="1">
-        <v>1.03058154365186E-8</v>
-      </c>
-      <c r="J72">
-        <v>0</v>
+        <v>6.2873727870719703E-9</v>
+      </c>
+      <c r="J72" s="1">
+        <v>4.8878481302112298E-11</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2.8113596911919501E-9</v>
+      </c>
+      <c r="C73" s="1">
+        <v>8.7211024432964898E-9</v>
+      </c>
+      <c r="D73" s="1">
+        <v>6.62989507356424E-9</v>
+      </c>
+      <c r="E73" s="1">
+        <v>9.1813788006872907E-9</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1.52400261368346E-8</v>
+      </c>
+      <c r="G73" s="1">
+        <v>7.5360529725183904E-8</v>
+      </c>
+      <c r="H73" s="1">
+        <v>2.8566357397374601E-9</v>
+      </c>
+      <c r="I73" s="1">
+        <v>1.03058154365186E-8</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>30</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73" s="1">
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1">
         <v>3.8217898894849803E-11</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D74" s="1">
         <v>5.2528340580726103E-9</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E74" s="1">
         <v>3.7208751524546802E-9</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F74" s="1">
         <v>8.3423906016789897E-8</v>
       </c>
-      <c r="G73" s="1">
+      <c r="G74" s="1">
         <v>3.4158602080085401E-9</v>
       </c>
-      <c r="H73" s="1">
+      <c r="H74" s="1">
         <v>1.6279963128819401E-10</v>
       </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="J73">
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J73">
-    <sortCondition ref="A2:A73"/>
+  <sortState ref="A2:J74">
+    <sortCondition ref="A2:A74"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>